<commit_message>
Mise à jour des tests
</commit_message>
<xml_diff>
--- a/doc/tests soamada.xlsx
+++ b/doc/tests soamada.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Nom du test</t>
   </si>
@@ -435,7 +435,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -508,11 +508,8 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
envois des mails, générations de fichiers PDF
</commit_message>
<xml_diff>
--- a/doc/tests soamada.xlsx
+++ b/doc/tests soamada.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="96" windowWidth="23784" windowHeight="10344" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="384" yWindow="96" windowWidth="23784" windowHeight="10344"/>
   </bookViews>
   <sheets>
     <sheet name="Test CU 1 Devenir membre" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="54">
   <si>
     <t>Nom du test</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>6. L'internaute visite le site notamment la page d'accueil où il y a la présentation de l'assocation, les projets, le formulaire de contact</t>
-  </si>
-  <si>
-    <t>Fonctionnalité nécessitant un déploiement</t>
   </si>
   <si>
     <t>1. Le membre clique sur le lien de connexion</t>
@@ -562,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -673,7 +670,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -698,55 +695,40 @@
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +750,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -790,7 +772,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -798,7 +780,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -806,7 +788,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -830,7 +812,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
@@ -838,7 +820,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
@@ -878,7 +860,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -886,7 +868,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -894,7 +876,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -918,7 +900,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
@@ -926,7 +908,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -966,7 +948,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -974,7 +956,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -982,7 +964,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -990,7 +972,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
@@ -998,7 +980,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -1006,18 +988,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
@@ -1025,7 +1007,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>10</v>
@@ -1042,7 +1024,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1047,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -1073,7 +1055,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -1081,7 +1063,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -1105,7 +1087,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
@@ -1120,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1144,7 +1126,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -1152,7 +1134,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -1160,7 +1142,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -1168,42 +1150,42 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>